<commit_message>
Extracted survey completion data from Survey Completion by Member and merged with May, June, July Email Event Listing.xlsx.
</commit_message>
<xml_diff>
--- a/May, June, July Email Event Listing.xlsx
+++ b/May, June, July Email Event Listing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lorio\OneDrive\Documents\Zensights\Email Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3EDD226-307B-4FED-925B-1782C04480BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{023D3A98-7865-421E-8636-EC6431461B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2091,8 +2091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D1105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
-      <selection activeCell="B89" sqref="B89"/>
+    <sheetView tabSelected="1" topLeftCell="A567" workbookViewId="0">
+      <selection activeCell="B525" sqref="B525"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -6078,7 +6078,7 @@
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A285" s="3">
-        <v>36892</v>
+        <v>45128</v>
       </c>
       <c r="B285" s="5" t="s">
         <v>82</v>
@@ -6162,7 +6162,7 @@
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A291" s="3">
-        <v>36892</v>
+        <v>45127</v>
       </c>
       <c r="B291" s="5" t="s">
         <v>88</v>
@@ -6176,7 +6176,7 @@
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A292" s="3">
-        <v>36892</v>
+        <v>45127</v>
       </c>
       <c r="B292" s="5" t="s">
         <v>80</v>
@@ -6190,7 +6190,7 @@
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A293" s="3">
-        <v>36892</v>
+        <v>45127</v>
       </c>
       <c r="B293" s="5" t="s">
         <v>76</v>
@@ -6204,7 +6204,7 @@
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A294" s="3">
-        <v>36892</v>
+        <v>45127</v>
       </c>
       <c r="B294" s="5" t="s">
         <v>23</v>
@@ -6232,7 +6232,7 @@
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A296" s="3">
-        <v>36892</v>
+        <v>45127</v>
       </c>
       <c r="B296" s="5" t="s">
         <v>15</v>
@@ -6260,7 +6260,7 @@
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A298" s="3">
-        <v>36892</v>
+        <v>45127</v>
       </c>
       <c r="B298" s="5" t="s">
         <v>535</v>
@@ -6274,7 +6274,7 @@
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A299" s="3">
-        <v>36892</v>
+        <v>45127</v>
       </c>
       <c r="B299" s="5" t="s">
         <v>91</v>
@@ -6288,7 +6288,7 @@
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A300" s="3">
-        <v>36892</v>
+        <v>45127</v>
       </c>
       <c r="B300" s="5" t="s">
         <v>93</v>
@@ -6302,7 +6302,7 @@
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A301" s="3">
-        <v>36892</v>
+        <v>45127</v>
       </c>
       <c r="B301" s="5" t="s">
         <v>95</v>
@@ -6316,7 +6316,7 @@
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A302" s="3">
-        <v>36892</v>
+        <v>45127</v>
       </c>
       <c r="B302" s="5" t="s">
         <v>536</v>
@@ -6330,7 +6330,7 @@
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A303" s="3">
-        <v>36892</v>
+        <v>45127</v>
       </c>
       <c r="B303" s="5" t="s">
         <v>536</v>
@@ -6344,7 +6344,7 @@
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A304" s="3">
-        <v>36892</v>
+        <v>45127</v>
       </c>
       <c r="B304" s="5" t="s">
         <v>98</v>
@@ -6358,7 +6358,7 @@
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A305" s="3">
-        <v>36892</v>
+        <v>45127</v>
       </c>
       <c r="B305" s="5" t="s">
         <v>100</v>
@@ -6372,7 +6372,7 @@
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A306" s="3">
-        <v>36892</v>
+        <v>45127</v>
       </c>
       <c r="B306" s="5" t="s">
         <v>86</v>
@@ -6386,7 +6386,7 @@
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A307" s="3">
-        <v>36892</v>
+        <v>45127</v>
       </c>
       <c r="B307" s="5" t="s">
         <v>86</v>
@@ -6400,7 +6400,7 @@
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A308" s="3">
-        <v>36892</v>
+        <v>45127</v>
       </c>
       <c r="B308" s="5" t="s">
         <v>91</v>
@@ -6526,7 +6526,7 @@
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A317" s="3">
-        <v>36892</v>
+        <v>45126</v>
       </c>
       <c r="B317" s="5" t="s">
         <v>91</v>
@@ -6610,7 +6610,7 @@
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A323" s="3">
-        <v>36892</v>
+        <v>45126</v>
       </c>
       <c r="B323" s="5" t="s">
         <v>122</v>
@@ -6624,7 +6624,7 @@
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A324" s="3">
-        <v>36892</v>
+        <v>45126</v>
       </c>
       <c r="B324" s="5" t="s">
         <v>86</v>
@@ -6652,7 +6652,7 @@
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A326" s="3">
-        <v>36892</v>
+        <v>45126</v>
       </c>
       <c r="B326" s="5" t="s">
         <v>126</v>
@@ -6680,7 +6680,7 @@
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A328" s="3">
-        <v>36892</v>
+        <v>45126</v>
       </c>
       <c r="B328" s="5" t="s">
         <v>130</v>
@@ -6722,7 +6722,7 @@
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A331" s="3">
-        <v>36892</v>
+        <v>45126</v>
       </c>
       <c r="B331" s="5" t="s">
         <v>130</v>
@@ -6792,7 +6792,7 @@
     </row>
     <row r="336" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A336" s="3">
-        <v>36892</v>
+        <v>45126</v>
       </c>
       <c r="B336" s="5" t="s">
         <v>106</v>
@@ -6820,7 +6820,7 @@
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A338" s="3">
-        <v>36892</v>
+        <v>45126</v>
       </c>
       <c r="B338" s="5" t="s">
         <v>134</v>
@@ -6834,7 +6834,7 @@
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A339" s="3">
-        <v>36892</v>
+        <v>45126</v>
       </c>
       <c r="B339" s="5" t="s">
         <v>106</v>
@@ -6848,7 +6848,7 @@
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A340" s="3">
-        <v>36892</v>
+        <v>45126</v>
       </c>
       <c r="B340" s="5" t="s">
         <v>102</v>
@@ -6862,7 +6862,7 @@
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A341" s="3">
-        <v>36892</v>
+        <v>45126</v>
       </c>
       <c r="B341" s="5" t="s">
         <v>136</v>
@@ -6876,7 +6876,7 @@
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A342" s="3">
-        <v>36892</v>
+        <v>45126</v>
       </c>
       <c r="B342" s="5" t="s">
         <v>138</v>
@@ -6890,7 +6890,7 @@
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A343" s="3">
-        <v>36892</v>
+        <v>45126</v>
       </c>
       <c r="B343" s="5" t="s">
         <v>140</v>
@@ -6918,7 +6918,7 @@
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A345" s="3">
-        <v>36892</v>
+        <v>45126</v>
       </c>
       <c r="B345" s="5" t="s">
         <v>144</v>
@@ -6946,7 +6946,7 @@
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A347" s="3">
-        <v>36892</v>
+        <v>45126</v>
       </c>
       <c r="B347" s="5" t="s">
         <v>146</v>
@@ -6988,7 +6988,7 @@
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A350" s="3">
-        <v>36892</v>
+        <v>45126</v>
       </c>
       <c r="B350" s="5" t="s">
         <v>148</v>
@@ -7030,7 +7030,7 @@
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A353" s="3">
-        <v>36892</v>
+        <v>45126</v>
       </c>
       <c r="B353" s="5" t="s">
         <v>155</v>
@@ -7058,7 +7058,7 @@
     </row>
     <row r="355" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A355" s="3">
-        <v>36892</v>
+        <v>45126</v>
       </c>
       <c r="B355" s="5" t="s">
         <v>159</v>
@@ -7086,7 +7086,7 @@
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A357" s="3">
-        <v>36892</v>
+        <v>45126</v>
       </c>
       <c r="B357" s="5" t="s">
         <v>155</v>
@@ -7114,7 +7114,7 @@
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A359" s="3">
-        <v>36892</v>
+        <v>45126</v>
       </c>
       <c r="B359" s="5" t="s">
         <v>163</v>
@@ -7142,7 +7142,7 @@
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A361" s="3">
-        <v>36892</v>
+        <v>45126</v>
       </c>
       <c r="B361" s="5" t="s">
         <v>165</v>
@@ -7268,7 +7268,7 @@
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A370" s="3">
-        <v>36892</v>
+        <v>45126</v>
       </c>
       <c r="B370" s="5" t="s">
         <v>537</v>
@@ -7296,7 +7296,7 @@
     </row>
     <row r="372" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A372" s="3">
-        <v>36892</v>
+        <v>45126</v>
       </c>
       <c r="B372" s="5" t="s">
         <v>178</v>
@@ -7310,7 +7310,7 @@
     </row>
     <row r="373" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A373" s="3">
-        <v>36892</v>
+        <v>45126</v>
       </c>
       <c r="B373" s="5" t="s">
         <v>172</v>
@@ -7338,7 +7338,7 @@
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A375" s="3">
-        <v>36892</v>
+        <v>45126</v>
       </c>
       <c r="B375" s="5" t="s">
         <v>182</v>
@@ -7366,7 +7366,7 @@
     </row>
     <row r="377" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A377" s="3">
-        <v>36892</v>
+        <v>45126</v>
       </c>
       <c r="B377" s="5" t="s">
         <v>184</v>
@@ -7394,7 +7394,7 @@
     </row>
     <row r="379" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A379" s="3">
-        <v>36892</v>
+        <v>45126</v>
       </c>
       <c r="B379" s="5" t="s">
         <v>188</v>
@@ -7436,7 +7436,7 @@
     </row>
     <row r="382" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A382" s="3">
-        <v>36892</v>
+        <v>45126</v>
       </c>
       <c r="B382" s="5" t="s">
         <v>188</v>
@@ -7464,7 +7464,7 @@
     </row>
     <row r="384" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A384" s="3">
-        <v>36892</v>
+        <v>45126</v>
       </c>
       <c r="B384" s="5" t="s">
         <v>192</v>
@@ -7492,7 +7492,7 @@
     </row>
     <row r="386" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A386" s="3">
-        <v>36892</v>
+        <v>45126</v>
       </c>
       <c r="B386" s="5" t="s">
         <v>76</v>
@@ -7520,7 +7520,7 @@
     </row>
     <row r="388" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A388" s="3">
-        <v>36892</v>
+        <v>45126</v>
       </c>
       <c r="B388" s="5" t="s">
         <v>192</v>
@@ -7548,7 +7548,7 @@
     </row>
     <row r="390" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A390" s="3">
-        <v>36892</v>
+        <v>45126</v>
       </c>
       <c r="B390" s="5" t="s">
         <v>73</v>
@@ -7926,7 +7926,7 @@
     </row>
     <row r="417" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A417" s="3">
-        <v>36892</v>
+        <v>45126</v>
       </c>
       <c r="B417" s="5" t="s">
         <v>222</v>
@@ -8094,7 +8094,7 @@
     </row>
     <row r="429" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A429" s="3">
-        <v>36892</v>
+        <v>45126</v>
       </c>
       <c r="B429" s="5" t="s">
         <v>230</v>
@@ -8248,7 +8248,7 @@
     </row>
     <row r="440" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A440" s="3">
-        <v>36892</v>
+        <v>45126</v>
       </c>
       <c r="B440" s="5" t="s">
         <v>210</v>
@@ -8262,7 +8262,7 @@
     </row>
     <row r="441" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A441" s="3">
-        <v>36892</v>
+        <v>45126</v>
       </c>
       <c r="B441" s="5" t="s">
         <v>238</v>
@@ -8276,7 +8276,7 @@
     </row>
     <row r="442" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A442" s="3">
-        <v>36892</v>
+        <v>45126</v>
       </c>
       <c r="B442" s="5" t="s">
         <v>234</v>
@@ -8290,7 +8290,7 @@
     </row>
     <row r="443" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A443" s="3">
-        <v>36892</v>
+        <v>45126</v>
       </c>
       <c r="B443" s="5" t="s">
         <v>21</v>
@@ -8304,7 +8304,7 @@
     </row>
     <row r="444" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A444" s="3">
-        <v>36892</v>
+        <v>45126</v>
       </c>
       <c r="B444" s="5" t="s">
         <v>240</v>
@@ -8416,7 +8416,7 @@
     </row>
     <row r="452" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A452" s="3">
-        <v>36892</v>
+        <v>45126</v>
       </c>
       <c r="B452" s="5" t="s">
         <v>224</v>
@@ -8444,7 +8444,7 @@
     </row>
     <row r="454" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A454" s="3">
-        <v>36892</v>
+        <v>45126</v>
       </c>
       <c r="B454" s="5" t="s">
         <v>245</v>

</xml_diff>